<commit_message>
Written new test cases
</commit_message>
<xml_diff>
--- a/HybridFramework_October/TestData/Data.xlsx
+++ b/HybridFramework_October/TestData/Data.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SauceLogin" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="webshop" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>UserName</t>
   </si>
@@ -28,13 +28,19 @@
   </si>
   <si>
     <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>dnr5dnr@gmail.com</t>
+  </si>
+  <si>
+    <t>Sample@1234</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,6 +62,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -74,15 +87,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -377,7 +396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -407,13 +426,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>